<commit_message>
rebuild to fix double counting bug
</commit_message>
<xml_diff>
--- a/RScripts/new_method/passenger breakdown.xlsx
+++ b/RScripts/new_method/passenger breakdown.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\creds2\LDT\RScripts\new_method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937411B6-C733-48ED-B97D-6D229EC19FBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1695" windowWidth="24120" windowHeight="13320" activeTab="1" xr2:uid="{2ABAB631-151F-4D81-947C-ECE6D8266FA8}"/>
+    <workbookView xWindow="1035" yWindow="1695" windowWidth="24120" windowHeight="13320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
     <sheet name="v2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="68">
   <si>
     <t>country</t>
   </si>
@@ -236,15 +235,6 @@
   </si>
   <si>
     <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>UK Domestic</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Slovakia</t>
   </si>
   <si>
     <t>Total</t>
@@ -253,7 +243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -322,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -361,6 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -675,7 +666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD7F64F-660A-4B07-A74F-F4087BD890F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1810,11 +1801,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289935C1-2527-486B-99B3-69EB41154F5B}">
-  <dimension ref="A1:R49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:H49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" activeCellId="1" sqref="B3:B6 B8:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,8 +1883,8 @@
         <v>52</v>
       </c>
       <c r="K2" s="6">
-        <f>SUM(B3:B20,F3:F21)</f>
-        <v>224119681</v>
+        <f>SUM(B3:B20,F3:F22)</f>
+        <v>224268744</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>50</v>
@@ -1923,32 +1914,32 @@
       </c>
       <c r="C3" s="11">
         <f>B3/$K$2 * 100</f>
-        <v>10.769901550948575</v>
+        <v>10.762743202414333</v>
       </c>
       <c r="D3" s="13">
         <v>35875214890.400002</v>
       </c>
       <c r="E3" s="11">
         <f>D3/$K$3 * 100</f>
-        <v>13.885679770757136</v>
+        <v>13.870601727537998</v>
       </c>
       <c r="F3" s="13">
         <v>19695510</v>
       </c>
       <c r="G3" s="11">
         <f>F3/$K$2 * 100</f>
-        <v>8.7879430811790247</v>
+        <v>8.782102065903576</v>
       </c>
       <c r="H3" s="13">
         <v>45020117312.400002</v>
       </c>
       <c r="I3" s="11">
         <f>H3/$K$3 * 100</f>
-        <v>17.425259588039104</v>
+        <v>17.406338021251536</v>
       </c>
       <c r="K3" s="6">
-        <f>SUM(D3:D20,H3:H21)</f>
-        <v>258361243256.89999</v>
+        <f>SUM(D3:D20,H3:H22)</f>
+        <v>258642094950.89999</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>51</v>
@@ -1978,28 +1969,28 @@
       </c>
       <c r="C4" s="11">
         <f t="shared" ref="C4:C20" si="0">B4/$K$2 * 100</f>
-        <v>6.1482141766924965</v>
+        <v>6.1441276899468438</v>
       </c>
       <c r="D4" s="13">
         <v>17342311367</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" ref="E4:E19" si="1">D4/$K$3 * 100</f>
-        <v>6.7124275871964958</v>
+        <v>6.7051387633912514</v>
       </c>
       <c r="F4" s="13">
         <v>2626357</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G21" si="2">F4/$K$2 * 100</f>
-        <v>1.1718546931181828</v>
+        <f t="shared" ref="G4:G22" si="2">F4/$K$2 * 100</f>
+        <v>1.1710758053739312</v>
       </c>
       <c r="H4" s="13">
         <v>4386891793.6999998</v>
       </c>
       <c r="I4" s="11">
-        <f t="shared" ref="I4:I21" si="3">H4/$K$3 * 100</f>
-        <v>1.6979682162846381</v>
+        <f t="shared" ref="I4:I22" si="3">H4/$K$3 * 100</f>
+        <v>1.6961244435221563</v>
       </c>
       <c r="N4" t="s">
         <v>3</v>
@@ -2026,28 +2017,28 @@
       </c>
       <c r="C5" s="11">
         <f t="shared" si="0"/>
-        <v>3.2191345123322752</v>
+        <v>3.2169948746848114</v>
       </c>
       <c r="D5" s="13">
         <v>12093992341.6</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="1"/>
-        <v>4.6810396904517173</v>
+        <v>4.6759566898404126</v>
       </c>
       <c r="F5" s="13">
         <v>962101</v>
       </c>
       <c r="G5" s="11">
         <f t="shared" si="2"/>
-        <v>0.42928001490417972</v>
+        <v>0.42899468862232537</v>
       </c>
       <c r="H5" s="13">
         <v>2269686950.6999998</v>
       </c>
       <c r="I5" s="11">
         <f t="shared" si="3"/>
-        <v>0.87849358599159155</v>
+        <v>0.87753965615336971</v>
       </c>
       <c r="N5" t="s">
         <v>4</v>
@@ -2070,32 +2061,32 @@
         <v>4</v>
       </c>
       <c r="B6" s="13">
-        <v>14770762</v>
+        <v>14795059</v>
       </c>
       <c r="C6" s="11">
         <f t="shared" si="0"/>
-        <v>6.5905689023357121</v>
+        <v>6.5970222760956831</v>
       </c>
       <c r="D6" s="13">
-        <v>11964543687.4</v>
+        <v>11984055274.700001</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="1"/>
-        <v>4.6309359471161571</v>
+        <v>4.6334512086963358</v>
       </c>
       <c r="F6" s="13">
-        <v>333943</v>
+        <v>309646</v>
       </c>
       <c r="G6" s="11">
         <f t="shared" si="2"/>
-        <v>0.14900208607739363</v>
+        <v>0.13806917293833867</v>
       </c>
       <c r="H6" s="13">
-        <v>253901085.69999999</v>
+        <v>234389498.40000001</v>
       </c>
       <c r="I6" s="11">
         <f t="shared" si="3"/>
-        <v>9.8273673906861841E-2</v>
+        <v>9.0623105432430073E-2</v>
       </c>
       <c r="N6" t="s">
         <v>66</v>
@@ -2115,35 +2106,35 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="13">
         <v>20504030</v>
       </c>
       <c r="C7" s="11">
         <f t="shared" si="0"/>
-        <v>9.1486967626015847</v>
+        <v>9.1426159679210581</v>
       </c>
       <c r="D7" s="13">
         <v>9946359961.5</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="1"/>
-        <v>3.8497879310829508</v>
+        <v>3.8456075618271628</v>
       </c>
       <c r="F7" s="13">
         <v>22464981</v>
       </c>
       <c r="G7" s="11">
         <f t="shared" si="2"/>
-        <v>10.023653835202452</v>
+        <v>10.016991489460519</v>
       </c>
       <c r="H7" s="13">
         <v>9227008017.3999996</v>
       </c>
       <c r="I7" s="11">
         <f t="shared" si="3"/>
-        <v>3.5713591950109862</v>
+        <v>3.5674811631693726</v>
       </c>
       <c r="N7" t="s">
         <v>5</v>
@@ -2170,28 +2161,28 @@
       </c>
       <c r="C8" s="11">
         <f t="shared" si="0"/>
-        <v>5.5753648872987647</v>
+        <v>5.5716591519324687</v>
       </c>
       <c r="D8" s="13">
         <v>9341122591.8999996</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>3.6155278067816501</v>
+        <v>3.6116018135691701</v>
       </c>
       <c r="F8" s="13">
         <v>997883</v>
       </c>
       <c r="G8" s="11">
         <f t="shared" si="2"/>
-        <v>0.44524559179610823</v>
+        <v>0.44494965379571572</v>
       </c>
       <c r="H8" s="13">
         <v>945727505.29999995</v>
       </c>
       <c r="I8" s="11">
         <f t="shared" si="3"/>
-        <v>0.36604851926634419</v>
+        <v>0.36565103815739458</v>
       </c>
       <c r="N8" t="s">
         <v>6</v>
@@ -2218,28 +2209,28 @@
       </c>
       <c r="C9" s="11">
         <f t="shared" si="0"/>
-        <v>2.7502399488066378</v>
+        <v>2.7484119677417018</v>
       </c>
       <c r="D9" s="13">
         <v>8557138815.8999996</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>3.3120829997676</v>
+        <v>3.3084865081704766</v>
       </c>
       <c r="F9" s="13">
         <v>1840311</v>
       </c>
       <c r="G9" s="11">
         <f t="shared" si="2"/>
-        <v>0.82112868972002517</v>
+        <v>0.82058291636038228</v>
       </c>
       <c r="H9" s="13">
         <v>2774574491.1999998</v>
       </c>
       <c r="I9" s="11">
         <f t="shared" si="3"/>
-        <v>1.0739128114665086</v>
+        <v>1.0727466817521403</v>
       </c>
       <c r="N9" t="s">
         <v>7</v>
@@ -2262,32 +2253,32 @@
         <v>7</v>
       </c>
       <c r="B10" s="13">
-        <v>5829765</v>
+        <v>5829808</v>
       </c>
       <c r="C10" s="11">
         <f t="shared" si="0"/>
-        <v>2.6011838737178996</v>
+        <v>2.5994741380457369</v>
       </c>
       <c r="D10" s="13">
-        <v>4777498445.6999998</v>
+        <v>4777533550.8999996</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="1"/>
-        <v>1.8491544573307082</v>
+        <v>1.8471600888505622</v>
       </c>
       <c r="F10" s="13">
-        <v>45314</v>
+        <v>45271</v>
       </c>
       <c r="G10" s="11">
         <f t="shared" si="2"/>
-        <v>2.0218661653369031E-2</v>
+        <v>2.0186049644082368E-2</v>
       </c>
       <c r="H10" s="13">
-        <v>51089812.299999997</v>
+        <v>51054707.100000001</v>
       </c>
       <c r="I10" s="11">
         <f t="shared" si="3"/>
-        <v>1.9774565122834285E-2</v>
+        <v>1.9739519628346695E-2</v>
       </c>
       <c r="N10" t="s">
         <v>8</v>
@@ -2314,28 +2305,28 @@
       </c>
       <c r="C11" s="11">
         <f t="shared" si="0"/>
-        <v>4.3985231265789642</v>
+        <v>4.3955995936732055</v>
       </c>
       <c r="D11" s="13">
         <v>4345049003.1000004</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>1.681772756751881</v>
+        <v>1.6799465701531895</v>
       </c>
       <c r="F11" s="13">
         <v>1139819</v>
       </c>
       <c r="G11" s="11">
         <f t="shared" si="2"/>
-        <v>0.50857604067355422</v>
+        <v>0.50823800930547858</v>
       </c>
       <c r="H11" s="13">
         <v>642751045.39999998</v>
       </c>
       <c r="I11" s="11">
         <f t="shared" si="3"/>
-        <v>0.24877997848960814</v>
+        <v>0.24850983577209981</v>
       </c>
       <c r="N11" t="s">
         <v>9</v>
@@ -2362,28 +2353,28 @@
       </c>
       <c r="C12" s="11">
         <f t="shared" si="0"/>
-        <v>1.223088926313437</v>
+        <v>1.2222759851011606</v>
       </c>
       <c r="D12" s="13">
         <v>3697553512.6999998</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
-        <v>1.4311564173049589</v>
+        <v>1.4296023674730653</v>
       </c>
       <c r="F12" s="13">
         <v>83711</v>
       </c>
       <c r="G12" s="11">
         <f t="shared" si="2"/>
-        <v>3.7351025856582405E-2</v>
+        <v>3.7326200034365917E-2</v>
       </c>
       <c r="H12" s="13">
         <v>118434017.09999999</v>
       </c>
       <c r="I12" s="11">
         <f t="shared" si="3"/>
-        <v>4.5840473442154722E-2</v>
+        <v>4.579069664684058E-2</v>
       </c>
       <c r="N12" t="s">
         <v>10</v>
@@ -2410,28 +2401,28 @@
       </c>
       <c r="C13" s="11">
         <f t="shared" si="0"/>
-        <v>1.4999454688675913</v>
+        <v>1.4989485115232999</v>
       </c>
       <c r="D13" s="13">
         <v>3208919068.5</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="1"/>
-        <v>1.2420280333258924</v>
+        <v>1.2406793523340327</v>
       </c>
       <c r="F13" s="13">
         <v>230591</v>
       </c>
       <c r="G13" s="11">
         <f t="shared" si="2"/>
-        <v>0.10288743896614773</v>
+        <v>0.10281905355478338</v>
       </c>
       <c r="H13" s="13">
         <v>197775259.90000001</v>
       </c>
       <c r="I13" s="11">
         <f t="shared" si="3"/>
-        <v>7.6549894793370127E-2</v>
+        <v>7.6466771558413651E-2</v>
       </c>
       <c r="N13" t="s">
         <v>58</v>
@@ -2451,35 +2442,35 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B14" s="13">
-        <v>2051200</v>
+        <v>1942055</v>
       </c>
       <c r="C14" s="11">
         <f t="shared" si="0"/>
-        <v>0.91522528983074891</v>
+        <v>0.86594991587414427</v>
       </c>
       <c r="D14" s="13">
-        <v>2246406408.0999999</v>
+        <v>2415556201</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="1"/>
-        <v>0.86948273656753494</v>
+        <v>0.93393776502566739</v>
       </c>
       <c r="F14" s="13">
-        <v>219179</v>
+        <v>453610</v>
       </c>
       <c r="G14" s="11">
         <f t="shared" si="2"/>
-        <v>9.7795516673076108E-2</v>
+        <v>0.20226180069033606</v>
       </c>
       <c r="H14" s="13">
-        <v>265867492.09999999</v>
+        <v>495954007</v>
       </c>
       <c r="I14" s="11">
         <f t="shared" si="3"/>
-        <v>0.10290533082612403</v>
+        <v>0.19175301185762153</v>
       </c>
       <c r="N14" t="s">
         <v>12</v>
@@ -2499,35 +2490,35 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B15" s="13">
-        <v>1566962</v>
+        <v>2051200</v>
       </c>
       <c r="C15" s="11">
         <f t="shared" si="0"/>
-        <v>0.69916305119138555</v>
+        <v>0.91461697399972952</v>
       </c>
       <c r="D15" s="13">
-        <v>2035994533</v>
+        <v>2246406408.0999999</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="1"/>
-        <v>0.78804177721637636</v>
+        <v>0.86853859134045919</v>
       </c>
       <c r="F15" s="13">
-        <v>828703</v>
+        <v>219179</v>
       </c>
       <c r="G15" s="11">
         <f t="shared" si="2"/>
-        <v>0.36975913775283303</v>
+        <v>9.773051567096662E-2</v>
       </c>
       <c r="H15" s="13">
-        <v>875515675</v>
+        <v>265867492.09999999</v>
       </c>
       <c r="I15" s="11">
         <f t="shared" si="3"/>
-        <v>0.33887268228131107</v>
+        <v>0.10279358901360264</v>
       </c>
       <c r="N15" t="s">
         <v>13</v>
@@ -2554,28 +2545,28 @@
       </c>
       <c r="C16" s="11">
         <f t="shared" si="0"/>
-        <v>0.75727530595583881</v>
+        <v>0.75677197353903225</v>
       </c>
       <c r="D16" s="13">
         <v>1998280766.9000001</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="1"/>
-        <v>0.77344447708552844</v>
+        <v>0.77260461692415106</v>
       </c>
       <c r="F16" s="13">
         <v>882901</v>
       </c>
       <c r="G16" s="11">
         <f t="shared" si="2"/>
-        <v>0.39394175293333566</v>
+        <v>0.39367991466523755</v>
       </c>
       <c r="H16" s="13">
         <v>865114721.70000005</v>
       </c>
       <c r="I16" s="11">
         <f t="shared" si="3"/>
-        <v>0.33484694174496532</v>
+        <v>0.33448334149328302</v>
       </c>
       <c r="N16" t="s">
         <v>14</v>
@@ -2602,28 +2593,28 @@
       </c>
       <c r="C17" s="11">
         <f t="shared" si="0"/>
-        <v>0.72493454959004688</v>
+        <v>0.72445271285774893</v>
       </c>
       <c r="D17" s="13">
         <v>787194176.20000005</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="1"/>
-        <v>0.30468740832666535</v>
+        <v>0.30435655740781065</v>
       </c>
       <c r="F17" s="13">
         <v>1363</v>
       </c>
       <c r="G17" s="11">
         <f t="shared" si="2"/>
-        <v>6.0815721043258142E-4</v>
+        <v>6.0775299120594353E-4</v>
       </c>
       <c r="H17" s="13">
         <v>1037239</v>
       </c>
       <c r="I17" s="11">
         <f t="shared" si="3"/>
-        <v>4.0146849694813839E-4</v>
+        <v>4.0103255434770089E-4</v>
       </c>
       <c r="N17" t="s">
         <v>15</v>
@@ -2646,14 +2637,14 @@
       </c>
       <c r="C18" s="11">
         <f t="shared" si="0"/>
-        <v>0.19417973381820047</v>
+        <v>0.19405066985170258</v>
       </c>
       <c r="D18" s="13">
         <v>760377641.5</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="1"/>
-        <v>0.29430793563101215</v>
+        <v>0.29398835547026797</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="11">
@@ -2683,35 +2674,35 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B19" s="13">
         <v>491099</v>
       </c>
       <c r="C19" s="11">
         <f t="shared" si="0"/>
-        <v>0.21912354943964069</v>
+        <v>0.2189779062569682</v>
       </c>
       <c r="D19" s="13">
         <v>672432357.70000005</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="1"/>
-        <v>0.26026827755716087</v>
+        <v>0.25998566004023937</v>
       </c>
       <c r="F19" s="13">
         <v>217538</v>
       </c>
       <c r="G19" s="11">
         <f t="shared" si="2"/>
-        <v>9.7063318593604453E-2</v>
+        <v>9.6998804256022406E-2</v>
       </c>
       <c r="H19" s="13">
         <v>338662391.39999998</v>
       </c>
       <c r="I19" s="11">
         <f t="shared" si="3"/>
-        <v>0.13108095747288731</v>
+        <v>0.13093862059240235</v>
       </c>
       <c r="N19" t="s">
         <v>17</v>
@@ -2738,28 +2729,28 @@
       </c>
       <c r="C20" s="11">
         <f t="shared" si="0"/>
-        <v>0.24756504985387695</v>
+        <v>0.24740050267548652</v>
       </c>
       <c r="D20" s="13">
         <v>281241825.39999998</v>
       </c>
       <c r="E20" s="11">
         <f>D20/$K$3 * 100</f>
-        <v>0.10885604274645359</v>
+        <v>0.10873783923432505</v>
       </c>
       <c r="F20" s="13">
         <v>470</v>
       </c>
       <c r="G20" s="11">
         <f t="shared" si="2"/>
-        <v>2.0970938290778668E-4</v>
+        <v>2.0956999696756674E-4</v>
       </c>
       <c r="H20" s="13">
         <v>287499</v>
       </c>
       <c r="I20" s="11">
         <f t="shared" si="3"/>
-        <v>1.1127791319463773E-4</v>
+        <v>1.1115707984602356E-4</v>
       </c>
       <c r="N20" t="s">
         <v>44</v>
@@ -2777,112 +2768,105 @@
       <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="14">
-        <f>SUM(F22:F48)</f>
-        <v>42271555</v>
+      <c r="C21" s="11"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="13">
+        <f>SUM(F22:F49)</f>
+        <v>42271752</v>
       </c>
       <c r="G21" s="11">
         <f t="shared" si="2"/>
-        <v>18.861152582133116</v>
-      </c>
-      <c r="H21" s="14">
-        <f t="shared" ref="H21" si="4">SUM(H22:H48)</f>
-        <v>60195169553.099998</v>
+        <v>18.848704124369643</v>
+      </c>
+      <c r="H21" s="13">
+        <f t="shared" ref="G21:I21" si="4">SUM(H22:H49)</f>
+        <v>60195590798.199997</v>
       </c>
       <c r="I21" s="11">
         <f t="shared" si="3"/>
-        <v>23.298838786452688</v>
-      </c>
-      <c r="N21" t="s">
-        <v>43</v>
-      </c>
-      <c r="O21" s="13">
-        <v>2948904</v>
-      </c>
+        <v>23.273702144125995</v>
+      </c>
+      <c r="O21" s="13"/>
       <c r="P21" s="13"/>
-      <c r="Q21" s="13">
-        <v>6026264567.6000004</v>
-      </c>
+      <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="13">
-        <v>7698601</v>
+        <v>26</v>
+      </c>
+      <c r="F22">
+        <v>148866</v>
       </c>
       <c r="G22" s="11"/>
-      <c r="H22" s="13">
-        <v>19455582647.700001</v>
+      <c r="H22">
+        <v>280430448.89999998</v>
       </c>
       <c r="I22" s="11"/>
       <c r="N22" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="O22" s="13">
-        <v>13008093</v>
+        <v>2948904</v>
       </c>
       <c r="P22" s="13"/>
       <c r="Q22" s="13">
-        <v>5551957120.3999996</v>
+        <v>6026264567.6000004</v>
       </c>
       <c r="R22" s="13"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="13">
-        <v>2948904</v>
+      <c r="F23">
+        <v>35011</v>
       </c>
       <c r="G23" s="11"/>
-      <c r="H23" s="13">
-        <v>6026264567.6000004</v>
+      <c r="H23">
+        <v>67636098.200000003</v>
       </c>
       <c r="I23" s="11"/>
       <c r="N23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="O23" s="13">
-        <v>1843155</v>
+        <v>13008093</v>
       </c>
       <c r="P23" s="13"/>
       <c r="Q23" s="13">
-        <v>4078521969</v>
+        <v>5551957120.3999996</v>
       </c>
       <c r="R23" s="13"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="13">
-        <v>13008093</v>
+      <c r="F24">
+        <v>197</v>
       </c>
       <c r="G24" s="11"/>
-      <c r="H24" s="13">
-        <v>5551957120.3999996</v>
+      <c r="H24">
+        <v>421245.1</v>
       </c>
       <c r="I24" s="11"/>
       <c r="N24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O24" s="13">
-        <v>1673142</v>
+        <v>1843155</v>
       </c>
       <c r="P24" s="13"/>
       <c r="Q24" s="13">
-        <v>3712611133.4000001</v>
+        <v>4078521969</v>
       </c>
       <c r="R24" s="13"/>
     </row>
@@ -2893,660 +2877,691 @@
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="13">
+      <c r="F25">
         <v>1843155</v>
       </c>
       <c r="G25" s="11"/>
-      <c r="H25" s="13">
+      <c r="H25">
         <v>4078521969</v>
       </c>
       <c r="I25" s="11"/>
       <c r="N25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O25" s="13">
-        <v>2256345</v>
+        <v>1673142</v>
       </c>
       <c r="P25" s="13"/>
       <c r="Q25" s="13">
-        <v>3475810112.5</v>
+        <v>3712611133.4000001</v>
       </c>
       <c r="R25" s="13"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="13">
-        <v>1673142</v>
+      <c r="F26">
+        <v>1661554</v>
       </c>
       <c r="G26" s="11"/>
-      <c r="H26" s="13">
-        <v>3712611133.4000001</v>
+      <c r="H26">
+        <v>2737106338.5</v>
       </c>
       <c r="I26" s="11"/>
       <c r="N26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O26" s="13">
-        <v>1601261</v>
+        <v>2256345</v>
       </c>
       <c r="P26" s="13"/>
       <c r="Q26" s="13">
-        <v>2877836350.6999998</v>
+        <v>3475810112.5</v>
       </c>
       <c r="R26" s="13"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="13">
-        <v>2256345</v>
+      <c r="F27">
+        <v>179785</v>
       </c>
       <c r="G27" s="11"/>
-      <c r="H27" s="13">
-        <v>3475810112.5</v>
+      <c r="H27">
+        <v>320216960.80000001</v>
       </c>
       <c r="I27" s="11"/>
       <c r="N27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O27" s="13">
-        <v>1661554</v>
+        <v>1601261</v>
       </c>
       <c r="P27" s="13"/>
       <c r="Q27" s="13">
-        <v>2737106338.5</v>
+        <v>2877836350.6999998</v>
       </c>
       <c r="R27" s="13"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="13">
-        <v>1601261</v>
+      <c r="F28">
+        <v>15810</v>
       </c>
       <c r="G28" s="11"/>
-      <c r="H28" s="13">
-        <v>2877836350.6999998</v>
+      <c r="H28">
+        <v>11443224.800000001</v>
       </c>
       <c r="I28" s="11"/>
       <c r="N28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O28" s="13">
-        <v>1407108</v>
+        <v>1661554</v>
       </c>
       <c r="P28" s="13"/>
       <c r="Q28" s="13">
-        <v>2678565769.1999998</v>
+        <v>2737106338.5</v>
       </c>
       <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="13">
-        <v>1661554</v>
+      <c r="F29">
+        <v>1407108</v>
       </c>
       <c r="G29" s="11"/>
-      <c r="H29" s="13">
-        <v>2737106338.5</v>
+      <c r="H29">
+        <v>2678565769.1999998</v>
       </c>
       <c r="I29" s="11"/>
       <c r="N29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O29" s="13">
-        <v>871345</v>
+        <v>1407108</v>
       </c>
       <c r="P29" s="13"/>
       <c r="Q29" s="13">
-        <v>2151236801.4000001</v>
+        <v>2678565769.1999998</v>
       </c>
       <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="13">
-        <v>1407108</v>
+      <c r="F30">
+        <v>7698601</v>
       </c>
       <c r="G30" s="11"/>
-      <c r="H30" s="13">
-        <v>2678565769.1999998</v>
+      <c r="H30">
+        <v>19455582647.700001</v>
       </c>
       <c r="I30" s="11"/>
       <c r="N30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O30" s="13">
-        <v>1181742</v>
+        <v>871345</v>
       </c>
       <c r="P30" s="13"/>
       <c r="Q30" s="13">
-        <v>2001773954.5</v>
+        <v>2151236801.4000001</v>
       </c>
       <c r="R30" s="13"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="13">
-        <v>871345</v>
+      <c r="F31">
+        <v>943393</v>
       </c>
       <c r="G31" s="11"/>
-      <c r="H31" s="13">
-        <v>2151236801.4000001</v>
+      <c r="H31">
+        <v>233490136.09999999</v>
       </c>
       <c r="I31" s="11"/>
       <c r="N31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O31" s="13">
-        <v>828698</v>
+        <v>1181742</v>
       </c>
       <c r="P31" s="13"/>
       <c r="Q31" s="13">
-        <v>1378449772.5999999</v>
+        <v>2001773954.5</v>
       </c>
       <c r="R31" s="13"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="13">
-        <v>1181742</v>
+      <c r="F32">
+        <v>2256345</v>
       </c>
       <c r="G32" s="11"/>
-      <c r="H32" s="13">
-        <v>2001773954.5</v>
+      <c r="H32">
+        <v>3475810112.5</v>
       </c>
       <c r="I32" s="11"/>
       <c r="N32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O32" s="13">
-        <v>399715</v>
+        <v>828698</v>
       </c>
       <c r="P32" s="13"/>
       <c r="Q32" s="13">
-        <v>854033657.29999995</v>
+        <v>1378449772.5999999</v>
       </c>
       <c r="R32" s="13"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="13">
-        <v>828698</v>
+      <c r="F33">
+        <v>1601261</v>
       </c>
       <c r="G33" s="11"/>
-      <c r="H33" s="13">
-        <v>1378449772.5999999</v>
+      <c r="H33">
+        <v>2877836350.6999998</v>
       </c>
       <c r="I33" s="11"/>
       <c r="N33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O33" s="13">
-        <v>2184049</v>
+        <v>399715</v>
       </c>
       <c r="P33" s="13"/>
       <c r="Q33" s="13">
-        <v>652053615.10000002</v>
+        <v>854033657.29999995</v>
       </c>
       <c r="R33" s="13"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="13">
-        <v>399715</v>
+      <c r="F34">
+        <v>13008093</v>
       </c>
       <c r="G34" s="11"/>
-      <c r="H34" s="13">
-        <v>854033657.29999995</v>
+      <c r="H34">
+        <v>5551957120.3999996</v>
       </c>
       <c r="I34" s="11"/>
       <c r="N34" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="O34" s="13">
-        <v>185029</v>
+        <v>2184049</v>
       </c>
       <c r="P34" s="13"/>
       <c r="Q34" s="13">
-        <v>400658718.19999999</v>
+        <v>652053615.10000002</v>
       </c>
       <c r="R34" s="13"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="13">
-        <v>2184049</v>
+      <c r="F35">
+        <v>546496</v>
       </c>
       <c r="G35" s="11"/>
-      <c r="H35" s="13">
-        <v>652053615.10000002</v>
+      <c r="H35">
+        <v>205786497.09999999</v>
       </c>
       <c r="I35" s="11"/>
       <c r="N35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O35" s="13">
-        <v>200227</v>
+        <v>185029</v>
       </c>
       <c r="P35" s="13"/>
       <c r="Q35" s="13">
-        <v>348089958.89999998</v>
+        <v>400658718.19999999</v>
       </c>
       <c r="R35" s="13"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="13">
-        <v>185029</v>
+      <c r="F36">
+        <v>2184049</v>
       </c>
       <c r="G36" s="11"/>
-      <c r="H36" s="13">
-        <v>400658718.19999999</v>
+      <c r="H36">
+        <v>652053615.10000002</v>
       </c>
       <c r="I36" s="11"/>
       <c r="N36" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="O36" s="13">
-        <v>179785</v>
+        <v>200227</v>
       </c>
       <c r="P36" s="13"/>
       <c r="Q36" s="13">
-        <v>320216960.80000001</v>
+        <v>348089958.89999998</v>
       </c>
       <c r="R36" s="13"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="13">
-        <v>200227</v>
+      <c r="F37">
+        <v>56374</v>
       </c>
       <c r="G37" s="11"/>
-      <c r="H37" s="13">
-        <v>348089958.89999998</v>
+      <c r="H37">
+        <v>107767996</v>
       </c>
       <c r="I37" s="11"/>
       <c r="N37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O37" s="13">
-        <v>250448</v>
+        <v>179785</v>
       </c>
       <c r="P37" s="13"/>
       <c r="Q37" s="13">
-        <v>306603305.89999998</v>
+        <v>320216960.80000001</v>
       </c>
       <c r="R37" s="13"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="13">
-        <v>179785</v>
+      <c r="F38">
+        <v>828698</v>
       </c>
       <c r="G38" s="11"/>
-      <c r="H38" s="13">
-        <v>320216960.80000001</v>
+      <c r="H38">
+        <v>1378449772.5999999</v>
       </c>
       <c r="I38" s="11"/>
       <c r="N38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O38" s="13">
-        <v>148866</v>
+        <v>250448</v>
       </c>
       <c r="P38" s="13"/>
       <c r="Q38" s="13">
-        <v>280430448.89999998</v>
+        <v>306603305.89999998</v>
       </c>
       <c r="R38" s="13"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
-      <c r="F39" s="13">
-        <v>250448</v>
+      <c r="F39">
+        <v>1181742</v>
       </c>
       <c r="G39" s="11"/>
-      <c r="H39" s="13">
-        <v>306603305.89999998</v>
+      <c r="H39">
+        <v>2001773954.5</v>
       </c>
       <c r="I39" s="11"/>
       <c r="N39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O39" s="13">
-        <v>943393</v>
+        <v>148866</v>
       </c>
       <c r="P39" s="13"/>
       <c r="Q39" s="13">
-        <v>233490136.09999999</v>
+        <v>280430448.89999998</v>
       </c>
       <c r="R39" s="13"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="13">
-        <v>148866</v>
+      <c r="F40">
+        <v>85330</v>
       </c>
       <c r="G40" s="11"/>
-      <c r="H40" s="13">
-        <v>280430448.89999998</v>
+      <c r="H40">
+        <v>170282318.5</v>
       </c>
       <c r="I40" s="11"/>
       <c r="N40" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="O40" s="13">
-        <v>546496</v>
+        <v>943393</v>
       </c>
       <c r="P40" s="13"/>
       <c r="Q40" s="13">
-        <v>205786497.09999999</v>
+        <v>233490136.09999999</v>
       </c>
       <c r="R40" s="13"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="13">
-        <v>943393</v>
+      <c r="F41">
+        <v>1673142</v>
       </c>
       <c r="G41" s="11"/>
-      <c r="H41" s="13">
-        <v>233490136.09999999</v>
+      <c r="H41">
+        <v>3712611133.4000001</v>
       </c>
       <c r="I41" s="11"/>
       <c r="N41" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="O41" s="13">
-        <v>85330</v>
+        <v>546496</v>
       </c>
       <c r="P41" s="13"/>
       <c r="Q41" s="13">
-        <v>170282318.5</v>
+        <v>205786497.09999999</v>
       </c>
       <c r="R41" s="13"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="13">
-        <v>546496</v>
+      <c r="F42">
+        <v>185029</v>
       </c>
       <c r="G42" s="11"/>
-      <c r="H42" s="13">
-        <v>205786497.09999999</v>
+      <c r="H42">
+        <v>400658718.19999999</v>
       </c>
       <c r="I42" s="11"/>
       <c r="N42" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="O42" s="13">
-        <v>60877</v>
+        <v>85330</v>
       </c>
       <c r="P42" s="13"/>
       <c r="Q42" s="13">
-        <v>110538834.7</v>
+        <v>170282318.5</v>
       </c>
       <c r="R42" s="13"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="13">
-        <v>85330</v>
+      <c r="F43">
+        <v>60877</v>
       </c>
       <c r="G43" s="11"/>
-      <c r="H43" s="13">
-        <v>170282318.5</v>
+      <c r="H43">
+        <v>110538834.7</v>
       </c>
       <c r="I43" s="11"/>
       <c r="N43" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="O43" s="13">
-        <v>56374</v>
+        <v>60877</v>
       </c>
       <c r="P43" s="13"/>
       <c r="Q43" s="13">
-        <v>107767996</v>
+        <v>110538834.7</v>
       </c>
       <c r="R43" s="13"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="13">
-        <v>60877</v>
+      <c r="F44">
+        <v>200227</v>
       </c>
       <c r="G44" s="11"/>
-      <c r="H44" s="13">
-        <v>110538834.7</v>
+      <c r="H44">
+        <v>348089958.89999998</v>
       </c>
       <c r="I44" s="11"/>
       <c r="N44" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O44" s="13">
-        <v>35011</v>
+        <v>56374</v>
       </c>
       <c r="P44" s="13"/>
       <c r="Q44" s="13">
-        <v>67636098.200000003</v>
+        <v>107767996</v>
       </c>
       <c r="R44" s="13"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="13">
-        <v>56374</v>
+      <c r="F45">
+        <v>2948904</v>
       </c>
       <c r="G45" s="11"/>
-      <c r="H45" s="13">
-        <v>107767996</v>
+      <c r="H45">
+        <v>6026264567.6000004</v>
       </c>
       <c r="I45" s="11"/>
       <c r="N45" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="O45" s="13">
-        <v>15810</v>
+        <v>35011</v>
       </c>
       <c r="P45" s="13"/>
       <c r="Q45" s="13">
-        <v>11443224.800000001</v>
+        <v>67636098.200000003</v>
       </c>
       <c r="R45" s="13"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
-      <c r="F46" s="13">
-        <v>35011</v>
+      <c r="F46">
+        <v>871345</v>
       </c>
       <c r="G46" s="11"/>
-      <c r="H46" s="13">
-        <v>67636098.200000003</v>
+      <c r="H46">
+        <v>2151236801.4000001</v>
       </c>
       <c r="I46" s="11"/>
       <c r="N46" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="O46" s="13">
-        <v>197</v>
+        <v>15810</v>
       </c>
       <c r="P46" s="13"/>
       <c r="Q46" s="13">
-        <v>421245.1</v>
+        <v>11443224.800000001</v>
       </c>
       <c r="R46" s="13"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="13">
-        <v>15810</v>
+      <c r="F47">
+        <v>250448</v>
       </c>
       <c r="G47" s="11"/>
-      <c r="H47" s="13">
-        <v>11443224.800000001</v>
+      <c r="H47">
+        <v>306603305.89999998</v>
       </c>
       <c r="I47" s="11"/>
+      <c r="N47" t="s">
+        <v>18</v>
+      </c>
+      <c r="O47" s="13">
+        <v>197</v>
+      </c>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13">
+        <v>421245.1</v>
+      </c>
+      <c r="R47" s="13"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
-      <c r="F48" s="13">
+      <c r="F48">
+        <v>399715</v>
+      </c>
+      <c r="G48" s="11"/>
+      <c r="H48">
+        <v>854033657.29999995</v>
+      </c>
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="13">
         <v>197</v>
       </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="13">
+      <c r="G49" s="11"/>
+      <c r="H49" s="13">
         <v>421245.1</v>
       </c>
-      <c r="I48" s="11"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" s="14">
-        <f>SUM(B22:B48,B3:B20)</f>
-        <v>129277451</v>
-      </c>
-      <c r="C49" s="14">
-        <f t="shared" ref="C49:H49" si="5">SUM(C22:C48,C3:C20)</f>
-        <v>57.682328666173682</v>
-      </c>
-      <c r="D49" s="14">
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="14">
+        <f>SUM(B22:B49,B3:B20)</f>
+        <v>129676884</v>
+      </c>
+      <c r="C50" s="16">
+        <f t="shared" ref="C50:I50" si="5">SUM(C22:C49,C3:C20)</f>
+        <v>57.822094014135118</v>
+      </c>
+      <c r="D50" s="14">
         <f t="shared" si="5"/>
-        <v>129931631394.49997</v>
-      </c>
-      <c r="E49" s="14">
+        <v>130330739754.99997</v>
+      </c>
+      <c r="E50" s="16">
         <f t="shared" si="5"/>
-        <v>50.290682052997873</v>
-      </c>
-      <c r="F49" s="14">
+        <v>50.390382037286578</v>
+      </c>
+      <c r="F50" s="14">
         <f t="shared" si="5"/>
-        <v>94842230</v>
-      </c>
-      <c r="G49" s="14">
+        <v>94442994</v>
+      </c>
+      <c r="G50" s="14">
         <f t="shared" si="5"/>
-        <v>23.456518751693217</v>
-      </c>
-      <c r="H49" s="14">
+        <v>23.262823463264237</v>
+      </c>
+      <c r="H50" s="14">
         <f t="shared" si="5"/>
-        <v>128429611862.39998</v>
+        <v>128030924746.99998</v>
+      </c>
+      <c r="I50" s="14">
+        <f t="shared" si="5"/>
+        <v>26.227491685635204</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:R46">
+  <sortState ref="N2:R46">
     <sortCondition descending="1" ref="R2:R46"/>
     <sortCondition descending="1" ref="Q2:Q46"/>
   </sortState>

</xml_diff>